<commit_message>
Upload new test steps.
</commit_message>
<xml_diff>
--- a/Moudle 6 Deliverables/DRAFT - Test Steps.xlsx
+++ b/Moudle 6 Deliverables/DRAFT - Test Steps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuseppevaccaro/Documents/GitHub/CS633---Term-Project/Moudle 6 Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E81E12A-E987-4A47-8C12-E39776623B84}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78042DB5-D161-AC42-BD34-FFAAD9493323}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" tabRatio="743" xr2:uid="{899C0D2E-80B1-AE45-A5B3-8AC8948BE8B6}"/>
   </bookViews>
@@ -1853,12 +1853,12 @@
   <dimension ref="B2:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>

</xml_diff>